<commit_message>
Added test case for new customer page
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Guru99BankData.xlsx
+++ b/src/test/resources/TestData/Guru99BankData.xlsx
@@ -4,28 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="240" windowWidth="28695" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="90" yWindow="240" windowWidth="28695" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTest" sheetId="2" r:id="rId1"/>
     <sheet name="HomePageTest" sheetId="3" r:id="rId2"/>
-    <sheet name="AddNewCustomerPage" sheetId="4" r:id="rId3"/>
+    <sheet name="NewCustomerPageTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>ExpectedResult</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>User or Password is not valid</t>
   </si>
@@ -79,13 +70,133 @@
   </si>
   <si>
     <t>Log out</t>
+  </si>
+  <si>
+    <t>verifyLinks</t>
+  </si>
+  <si>
+    <t>addCustomerHeading</t>
+  </si>
+  <si>
+    <t>verifyAddNewCustomerHeading</t>
+  </si>
+  <si>
+    <t>Add New Customer</t>
+  </si>
+  <si>
+    <t>verifyCustomerNameLabel</t>
+  </si>
+  <si>
+    <t>customerNameLabel</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>verifyGenderLabel</t>
+  </si>
+  <si>
+    <t>genderLabel</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>verifyDOBLabel</t>
+  </si>
+  <si>
+    <t>dobLabel</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>verifyAddressLabel</t>
+  </si>
+  <si>
+    <t>addressLabel</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>verifyCityLabel</t>
+  </si>
+  <si>
+    <t>cityLabel</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>verifyStateLabel</t>
+  </si>
+  <si>
+    <t>stateLabel</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>verifyPINLabel</t>
+  </si>
+  <si>
+    <t>pinLabel</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>verifyMobileNumberLabel</t>
+  </si>
+  <si>
+    <t>Mobile Number</t>
+  </si>
+  <si>
+    <t>verifyEmailLabel</t>
+  </si>
+  <si>
+    <t>emailLabel</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>verifyPasswordLabel</t>
+  </si>
+  <si>
+    <t>passwordLabel</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>mobileNumberLabel</t>
+  </si>
+  <si>
+    <t>verifyUserIdLabelText</t>
+  </si>
+  <si>
+    <t>userIdLabel</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>verifyPasswordLabelText</t>
+  </si>
+  <si>
+    <t>verifyJavascriptAlertText</t>
+  </si>
+  <si>
+    <t>alertText</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +204,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,7 +221,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,9 +250,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +567,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -425,173 +641,141 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="6">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="6">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -602,14 +786,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1">
+      <c r="A1" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="1" customFormat="1">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="1" customFormat="1">
+      <c r="A9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="1" customFormat="1">
+      <c r="A13" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="1" customFormat="1">
+      <c r="A17" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="1" customFormat="1">
+      <c r="A21" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="1" customFormat="1">
+      <c r="A25" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="1" customFormat="1">
+      <c r="A29" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="1" customFormat="1">
+      <c r="A33" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" s="1" customFormat="1">
+      <c r="A37" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" s="1" customFormat="1">
+      <c r="A41" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>